<commit_message>
Completed the data sheet
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\leipzig-map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8330DA6-5A09-4D47-8383-4F2790D61B96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A419A6-1444-4CD7-8B86-CFAC35541758}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -310,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -319,7 +319,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -630,8 +634,8 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,11 +675,11 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>51.202167000000003</v>
-      </c>
-      <c r="C2" s="4">
-        <v>12.222161</v>
+      <c r="B2" s="4">
+        <v>51.339237199999999</v>
+      </c>
+      <c r="C2" s="5">
+        <v>12.3757456</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -694,11 +698,11 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>51.201996999999999</v>
-      </c>
-      <c r="C3" s="3">
-        <v>12.222785</v>
+      <c r="B3" s="4">
+        <v>51.338879599999999</v>
+      </c>
+      <c r="C3" s="6">
+        <v>12.3744023</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -717,11 +721,11 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>51.194093000000002</v>
-      </c>
-      <c r="C4" s="3">
-        <v>12.194787</v>
+      <c r="B4" s="4">
+        <v>51.328572600000001</v>
+      </c>
+      <c r="C4" s="6">
+        <v>12.331050899999999</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>51</v>
@@ -740,11 +744,11 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5">
-        <v>51194779</v>
-      </c>
-      <c r="C5" s="3">
-        <v>12.201489</v>
+      <c r="B5" s="4">
+        <v>51.330156500000001</v>
+      </c>
+      <c r="C5" s="6">
+        <v>12.337664800000001</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>47</v>
@@ -763,11 +767,11 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
-        <v>5120091</v>
-      </c>
-      <c r="C6" s="3">
-        <v>12.202067</v>
+      <c r="B6" s="4">
+        <v>51.3332081</v>
+      </c>
+      <c r="C6" s="6">
+        <v>12.3392631</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>49</v>
@@ -786,11 +790,11 @@
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
-        <v>51.195771000000001</v>
-      </c>
-      <c r="C7" s="3">
-        <v>12.201846</v>
+      <c r="B7" s="4">
+        <v>51.332988299999997</v>
+      </c>
+      <c r="C7" s="6">
+        <v>12.337859999999999</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>50</v>
@@ -809,11 +813,11 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
-        <v>51.195843000000004</v>
-      </c>
-      <c r="C8" s="3">
-        <v>12.20213</v>
+      <c r="B8" s="4">
+        <v>51.332929900000003</v>
+      </c>
+      <c r="C8" s="6">
+        <v>12.3397963</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>48</v>
@@ -832,11 +836,11 @@
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9">
-        <v>51.19171</v>
-      </c>
-      <c r="C9" s="3">
-        <v>12.223189</v>
+      <c r="B9" s="4">
+        <v>51.317073200000003</v>
+      </c>
+      <c r="C9" s="6">
+        <v>12.3754904</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
@@ -855,11 +859,11 @@
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10">
-        <v>51.193821</v>
-      </c>
-      <c r="C10" s="3">
-        <v>12.2224</v>
+      <c r="B10" s="4">
+        <v>51.327552400000002</v>
+      </c>
+      <c r="C10" s="6">
+        <v>12.373935700000001</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>22</v>
@@ -878,11 +882,11 @@
       <c r="A11" t="s">
         <v>63</v>
       </c>
-      <c r="B11">
-        <v>51.195889999999999</v>
-      </c>
-      <c r="C11" s="3">
-        <v>12.222624</v>
+      <c r="B11" s="4">
+        <v>51.332919199999999</v>
+      </c>
+      <c r="C11" s="6">
+        <v>12.373799099999999</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>52</v>
@@ -901,11 +905,11 @@
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12">
-        <v>51.202159000000002</v>
-      </c>
-      <c r="C12" s="3">
-        <v>12.212476000000001</v>
+      <c r="B12" s="4">
+        <v>51.339290499999997</v>
+      </c>
+      <c r="C12" s="6">
+        <v>12.3581936</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>53</v>
@@ -924,11 +928,11 @@
       <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13">
-        <v>51.202258</v>
-      </c>
-      <c r="C13" s="3">
-        <v>12.215835999999999</v>
+      <c r="B13" s="4">
+        <v>51.339855</v>
+      </c>
+      <c r="C13" s="6">
+        <v>12.3674306</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>54</v>
@@ -947,11 +951,11 @@
       <c r="A14" t="s">
         <v>29</v>
       </c>
-      <c r="B14">
-        <v>51.202688999999999</v>
-      </c>
-      <c r="C14" s="3">
-        <v>12.222358</v>
+      <c r="B14" s="4">
+        <v>51.340958200000003</v>
+      </c>
+      <c r="C14" s="6">
+        <v>12.373424</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>55</v>
@@ -970,11 +974,11 @@
       <c r="A15" t="s">
         <v>31</v>
       </c>
-      <c r="B15">
-        <v>51.20411</v>
-      </c>
-      <c r="C15" s="3">
-        <v>12.222419</v>
+      <c r="B15" s="4">
+        <v>51.344570400000002</v>
+      </c>
+      <c r="C15" s="6">
+        <v>12.374700900000001</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>32</v>
@@ -993,11 +997,11 @@
       <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16">
-        <v>51.204341999999997</v>
-      </c>
-      <c r="C16" s="3">
-        <v>12.221363</v>
+      <c r="B16" s="4">
+        <v>51.3451278</v>
+      </c>
+      <c r="C16" s="6">
+        <v>12.3709808</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>68</v>
@@ -1016,11 +1020,11 @@
       <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="B17">
-        <v>51.204410000000003</v>
-      </c>
-      <c r="C17" s="3">
-        <v>12.221439999999999</v>
+      <c r="B17" s="4">
+        <v>51.344601400000002</v>
+      </c>
+      <c r="C17" s="6">
+        <v>12.3710349</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>36</v>
@@ -1039,11 +1043,11 @@
       <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="B18">
-        <v>51.202582</v>
-      </c>
-      <c r="C18" s="3">
-        <v>12.224629999999999</v>
+      <c r="B18" s="4">
+        <v>51.3404673</v>
+      </c>
+      <c r="C18" s="6">
+        <v>12.379617700000001</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>39</v>
@@ -1062,11 +1066,11 @@
       <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="B19">
-        <v>51.201497000000003</v>
-      </c>
-      <c r="C19" s="3">
-        <v>12.225390000000001</v>
+      <c r="B19" s="4">
+        <v>51.337847600000003</v>
+      </c>
+      <c r="C19" s="6">
+        <v>12.3814378</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>42</v>
@@ -1085,11 +1089,11 @@
       <c r="A20" t="s">
         <v>44</v>
       </c>
-      <c r="B20">
-        <v>51.2042</v>
-      </c>
-      <c r="C20" s="3">
-        <v>12.232647</v>
+      <c r="B20" s="4">
+        <v>51.345033000000001</v>
+      </c>
+      <c r="C20" s="6">
+        <v>12.3906513</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>56</v>
@@ -1108,11 +1112,11 @@
       <c r="A21" t="s">
         <v>45</v>
       </c>
-      <c r="B21">
-        <v>51.202001000000003</v>
-      </c>
-      <c r="C21" s="3">
-        <v>12.23372</v>
+      <c r="B21" s="4">
+        <v>51.3390968</v>
+      </c>
+      <c r="C21" s="6">
+        <v>12.393767499999999</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>46</v>
@@ -1131,11 +1135,11 @@
       <c r="A22" t="s">
         <v>57</v>
       </c>
-      <c r="B22">
-        <v>51.204222999999999</v>
-      </c>
-      <c r="C22" s="3">
-        <v>12.215728</v>
+      <c r="B22" s="4">
+        <v>51.344477099999999</v>
+      </c>
+      <c r="C22" s="6">
+        <v>12.366763000000001</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>58</v>
@@ -1154,11 +1158,11 @@
       <c r="A23" t="s">
         <v>59</v>
       </c>
-      <c r="B23">
-        <v>51.195722000000004</v>
-      </c>
-      <c r="C23" s="3">
-        <v>12.222416000000001</v>
+      <c r="B23" s="4">
+        <v>51.331298599999997</v>
+      </c>
+      <c r="C23" s="6">
+        <v>12.374067699999999</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>60</v>
@@ -1177,11 +1181,11 @@
       <c r="A24" t="s">
         <v>61</v>
       </c>
-      <c r="B24">
-        <v>51.195917000000001</v>
-      </c>
-      <c r="C24" s="3">
-        <v>12.214267</v>
+      <c r="B24" s="4">
+        <v>51.333154299999997</v>
+      </c>
+      <c r="C24" s="6">
+        <v>12.3622513</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>62</v>
@@ -1200,11 +1204,11 @@
       <c r="A25" t="s">
         <v>64</v>
       </c>
-      <c r="B25">
-        <v>51.193671999999999</v>
-      </c>
-      <c r="C25" s="3">
-        <v>12.221743999999999</v>
+      <c r="B25" s="4">
+        <v>51.325598300000003</v>
+      </c>
+      <c r="C25" s="6">
+        <v>12.371049899999999</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>65</v>
@@ -1223,11 +1227,11 @@
       <c r="A26" t="s">
         <v>76</v>
       </c>
-      <c r="B26">
-        <v>51.192393000000003</v>
-      </c>
-      <c r="C26" s="3">
-        <v>12.222356</v>
+      <c r="B26" s="4">
+        <v>51.323686600000002</v>
+      </c>
+      <c r="C26" s="6">
+        <v>12.372990400000001</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
Remove some unneeded comments
</commit_message>
<xml_diff>
--- a/raw_data.xlsx
+++ b/raw_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\leipzig-map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\work\leipzig-map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A419A6-1444-4CD7-8B86-CFAC35541758}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69F34D2-E35F-4D2D-AD94-D5446A238C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>Schreberverein</t>
   </si>
   <si>
-    <t>http://www.schreber-leipzig.de/images/Historie/Vereinshaus/Bauzeichnung.jpg</t>
-  </si>
-  <si>
     <t>Odeon</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t xml:space="preserve">Auf dem Gelände der heutigen Dresdner Straße 20 befand sich das 1838 errichtete Gasthaus "Colosseum", das 1863 in "Pantheon" umbenannt wurde. 1848 wurde hier durch Auguste Schmidt der "Verein der Dienstmädchen" als erste Frauen-Berufsorganisation gegründet. Am 23.05.1863 fand hier die Gründung des Allgemeinen Deutschen Arbeitervereins (ADAV) durch Ferdinand Lassalle und Arbeitervertreter aus 12 deutschen Städten statt. Somit zählt der Ort neben dem Goldenen Löwen in Eisenach und dem Tivoli in Gotha zu den drei Gründungsorten der deutschen Sozialdemokratie. Hier traten u. a. August Bebel (1891), Clara Zetkin (1893), Wilhelm Liebknecht (1893) und Karl Liebknecht (1900) als Redner auf, Clara Zetkin sprach hier über "Die Frauen des Proletariats und der Militarismus". Zudem wurde hier 1891 die erste offizielle Leipziger Maifeier initiiert. 1918/19 wurde in dem Gebäude ein Kino eingerichtet (UT Dresdner Straße). 1933 wurde der Versammlungssaal, 1977 auch das Vorderhaus abgerissen. Heute erinnert nur ein 2013 verlegter Gedenkstein an die Bedeutung des Ortes. </t>
   </si>
   <si>
-    <t>Am 28.10.1900 eröffnet (heute Zschocherschen Straße 41a). Eines der anschaulichsten Beispiele für die zahlreichen Warenhäuser des Consum-Vereins, die sich zu Beginn des 20. Jh. über die gesamte Stadt verteilten.</t>
-  </si>
-  <si>
     <t>In diesem um 1860 errichteten Wohnhaus mit Garten wohnte seit 1909 die Familie Zeigner. Nach der Scheidung seiner ersten Ehe zog Erich Zeigner wieder in die Wohnung seiner Eltern, die sich im Erdgeschoss links des Wohnungseingangs befand. Anlässlich seiner Einsetzung als Leipziger Oberbürgermeister 1945 wurde das gesamte Erdgeschoss zu seiner Wohnung um- und ausgebaut. Nach seinem frühen Tod 1949 wurde die originale Wohnungseinrichtung durch seine zweite Ehefrau Annemarie weitestgehend bewahrt. Seine Sekretärin Johanna Landgraf wohnte noch bis zu ihrem Tod 2012 im Haus. Heute wird das Haus durch den Erich-Zeigner-Verein für politische Bildungsveranstaltungen genutzt.</t>
   </si>
   <si>
@@ -266,6 +260,12 @@
   </si>
   <si>
     <t>privat</t>
+  </si>
+  <si>
+    <t>Am 28.10.1900 eröffnet (heute Zschochersche Straße 41a). Eines der anschaulichsten Beispiele für die zahlreichen Warenhäuser des Consum-Vereins, die sich zu Beginn des 20. Jh. über die gesamte Stadt verteilten.</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/4/4e/Deutsches_Kleing%C3%A4rtnermuseum_Leipzig_2011.jpg</t>
   </si>
 </sst>
 </file>
@@ -310,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -319,11 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -635,20 +631,20 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="174" style="2" customWidth="1"/>
-    <col min="5" max="5" width="57.88671875" customWidth="1"/>
+    <col min="5" max="5" width="57.85546875" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -668,40 +664,40 @@
         <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2">
         <v>51.339237199999999</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>12.3757456</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>51.338879599999999</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>12.3744023</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -711,135 +707,135 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4">
         <v>51.328572600000001</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>12.331050899999999</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5">
         <v>51.330156500000001</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="3">
         <v>12.337664800000001</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6">
         <v>51.3332081</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="3">
         <v>12.3392631</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7">
         <v>51.332988299999997</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>12.337859999999999</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8">
         <v>51.332929900000003</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>12.3397963</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9">
         <v>51.317073200000003</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="3">
         <v>12.3754904</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -849,20 +845,20 @@
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10">
         <v>51.327552400000002</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="3">
         <v>12.373935700000001</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -872,378 +868,378 @@
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="4">
+        <v>61</v>
+      </c>
+      <c r="B11">
         <v>51.332919199999999</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="3">
         <v>12.373799099999999</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
         <v>51.339290499999997</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="3">
         <v>12.3581936</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>51.339855</v>
+      </c>
+      <c r="C13" s="3">
+        <v>12.3674306</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>51.340958200000003</v>
+      </c>
+      <c r="C14" s="3">
+        <v>12.373424</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>51.344570400000002</v>
+      </c>
+      <c r="C15" s="3">
+        <v>12.374700900000001</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16">
+        <v>51.3451278</v>
+      </c>
+      <c r="C16" s="3">
+        <v>12.3709808</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17">
+        <v>51.344601400000002</v>
+      </c>
+      <c r="C17" s="3">
+        <v>12.3710349</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="G17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18">
+        <v>51.3404673</v>
+      </c>
+      <c r="C18" s="3">
+        <v>12.379617700000001</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <v>51.337847600000003</v>
+      </c>
+      <c r="C19" s="3">
+        <v>12.3814378</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20">
+        <v>51.345033000000001</v>
+      </c>
+      <c r="C20" s="3">
+        <v>12.3906513</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" t="s">
         <v>70</v>
       </c>
-      <c r="G12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="4">
-        <v>51.339855</v>
-      </c>
-      <c r="C13" s="6">
-        <v>12.3674306</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21">
+        <v>51.3390968</v>
+      </c>
+      <c r="C21" s="3">
+        <v>12.393767499999999</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22">
+        <v>51.344477099999999</v>
+      </c>
+      <c r="C22" s="3">
+        <v>12.366763000000001</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" t="s">
         <v>70</v>
       </c>
-      <c r="G13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="4">
-        <v>51.340958200000003</v>
-      </c>
-      <c r="C14" s="6">
-        <v>12.373424</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="4">
-        <v>51.344570400000002</v>
-      </c>
-      <c r="C15" s="6">
-        <v>12.374700900000001</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="4">
-        <v>51.3451278</v>
-      </c>
-      <c r="C16" s="6">
-        <v>12.3709808</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="G22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
+        <v>51.331298599999997</v>
+      </c>
+      <c r="C23" s="3">
+        <v>12.374067699999999</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F16" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="4">
-        <v>51.344601400000002</v>
-      </c>
-      <c r="C17" s="6">
-        <v>12.3710349</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="4">
-        <v>51.3404673</v>
-      </c>
-      <c r="C18" s="6">
-        <v>12.379617700000001</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="4">
-        <v>51.337847600000003</v>
-      </c>
-      <c r="C19" s="6">
-        <v>12.3814378</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="4">
-        <v>51.345033000000001</v>
-      </c>
-      <c r="C20" s="6">
-        <v>12.3906513</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="F23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24">
+        <v>51.333154299999997</v>
+      </c>
+      <c r="C24" s="3">
+        <v>12.3622513</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G20" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="4">
-        <v>51.3390968</v>
-      </c>
-      <c r="C21" s="6">
-        <v>12.393767499999999</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="4">
-        <v>51.344477099999999</v>
-      </c>
-      <c r="C22" s="6">
-        <v>12.366763000000001</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="4">
-        <v>51.331298599999997</v>
-      </c>
-      <c r="C23" s="6">
-        <v>12.374067699999999</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="F24" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25">
+        <v>51.325598300000003</v>
+      </c>
+      <c r="C25" s="3">
+        <v>12.371049899999999</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F23" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="4">
-        <v>51.333154299999997</v>
-      </c>
-      <c r="C24" s="6">
-        <v>12.3622513</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="F25" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>74</v>
       </c>
-      <c r="F24" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="4">
-        <v>51.325598300000003</v>
-      </c>
-      <c r="C25" s="6">
-        <v>12.371049899999999</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="B26">
+        <v>51.323686600000002</v>
+      </c>
+      <c r="C26" s="3">
+        <v>12.372990400000001</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G25" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="E26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="4">
-        <v>51.323686600000002</v>
-      </c>
-      <c r="C26" s="6">
-        <v>12.372990400000001</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>